<commit_message>
add new MA data source
</commit_message>
<xml_diff>
--- a/tableau/state_info.xlsx
+++ b/tableau/state_info.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andy/Documents/GitHub/coronavirus-unemployment/tableau/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90BEC51-0593-984E-A0D3-9AAF9F53F7DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0814DCB9-D9DD-D347-8C7A-E8A3F56239EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{FAAD1E06-CFD9-6944-82C2-576030DD8CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="276">
   <si>
     <t>State</t>
   </si>
@@ -524,9 +524,6 @@
     <t>Department of Unemployment Assistance, Economic Research, Workforce Development Area Profile</t>
   </si>
   <si>
-    <t>https://public.tableau.com/profile/maeconomicresearch#!/vizhome/WorkforceDevelopmentAreaWDAProfile/WDAProfile</t>
-  </si>
-  <si>
     <t>https://lmi.dua.eol.mass.gov/LMI/LaborForceAndUnemployment#</t>
   </si>
   <si>
@@ -852,6 +849,18 @@
   </si>
   <si>
     <t>Unemployment Insurance data for Connecticut is available on a weekly basis. Unemployment data is available at the state, county, and city levels.</t>
+  </si>
+  <si>
+    <t>https://public.tableau.com/profile/louisiana.workforce.commission.lmi#!/vizhome/LWCUIDashboard/DashboardMain</t>
+  </si>
+  <si>
+    <t>Louisiana Workforce Commission, UI Claims by Parish</t>
+  </si>
+  <si>
+    <t>https://public.tableau.com/profile/maeconomicresearch#!/vizhome/InitialClaimsbyCounty_15943981899640/GenderRaceEthnicitybyCounty</t>
+  </si>
+  <si>
+    <t>Department of Unemployment Assistance, Economic Research, Initial Claims by County</t>
   </si>
 </sst>
 </file>
@@ -1222,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9EF56E-AA8C-6C43-9629-B47516959724}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1285,7 +1294,7 @@
         <v>105</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1299,13 +1308,13 @@
         <v>111</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E4" t="s">
         <v>110</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1359,7 +1368,7 @@
         <v>120</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1367,13 +1376,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E8" t="s">
         <v>122</v>
@@ -1501,7 +1510,7 @@
         <v>143</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1541,7 +1550,7 @@
         <v>150</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1571,11 +1580,17 @@
       <c r="B19" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="C19" t="s">
+        <v>273</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="E19" t="s">
         <v>155</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1620,16 +1635,16 @@
         <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>162</v>
+        <v>275</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E22" t="s">
+        <v>164</v>
+      </c>
+      <c r="F22" t="s">
         <v>163</v>
-      </c>
-      <c r="E22" t="s">
-        <v>165</v>
-      </c>
-      <c r="F22" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1640,16 +1655,16 @@
         <v>71</v>
       </c>
       <c r="C23" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E23" t="s">
+        <v>168</v>
+      </c>
+      <c r="F23" t="s">
         <v>167</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E23" t="s">
-        <v>169</v>
-      </c>
-      <c r="F23" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1660,16 +1675,16 @@
         <v>72</v>
       </c>
       <c r="C24" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E24" t="s">
         <v>171</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="F24" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1680,16 +1695,16 @@
         <v>73</v>
       </c>
       <c r="C25" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25" t="s">
         <v>174</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>176</v>
+      </c>
+      <c r="F25" t="s">
         <v>175</v>
-      </c>
-      <c r="E25" t="s">
-        <v>177</v>
-      </c>
-      <c r="F25" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1700,16 +1715,16 @@
         <v>74</v>
       </c>
       <c r="C26" t="s">
+        <v>177</v>
+      </c>
+      <c r="D26" t="s">
         <v>178</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>179</v>
       </c>
-      <c r="E26" t="s">
-        <v>180</v>
-      </c>
       <c r="F26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1720,10 +1735,10 @@
         <v>75</v>
       </c>
       <c r="E27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1734,16 +1749,16 @@
         <v>76</v>
       </c>
       <c r="C28" t="s">
+        <v>183</v>
+      </c>
+      <c r="D28" t="s">
         <v>184</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
+        <v>186</v>
+      </c>
+      <c r="F28" t="s">
         <v>185</v>
-      </c>
-      <c r="E28" t="s">
-        <v>187</v>
-      </c>
-      <c r="F28" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1754,16 +1769,16 @@
         <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E29" t="s">
+        <v>197</v>
+      </c>
+      <c r="F29" t="s">
         <v>188</v>
-      </c>
-      <c r="E29" t="s">
-        <v>198</v>
-      </c>
-      <c r="F29" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1774,10 +1789,10 @@
         <v>78</v>
       </c>
       <c r="E30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1788,16 +1803,16 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
+        <v>191</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E31" t="s">
         <v>192</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="E31" t="s">
-        <v>193</v>
-      </c>
       <c r="F31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1808,16 +1823,16 @@
         <v>80</v>
       </c>
       <c r="C32" t="s">
+        <v>193</v>
+      </c>
+      <c r="D32" t="s">
         <v>194</v>
       </c>
-      <c r="D32" t="s">
-        <v>195</v>
-      </c>
       <c r="E32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1828,16 +1843,16 @@
         <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D33" t="s">
+        <v>200</v>
+      </c>
+      <c r="E33" t="s">
+        <v>204</v>
+      </c>
+      <c r="F33" t="s">
         <v>201</v>
-      </c>
-      <c r="E33" t="s">
-        <v>205</v>
-      </c>
-      <c r="F33" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1848,10 +1863,10 @@
         <v>82</v>
       </c>
       <c r="E34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1862,16 +1877,16 @@
         <v>83</v>
       </c>
       <c r="C35" t="s">
+        <v>213</v>
+      </c>
+      <c r="D35" t="s">
+        <v>206</v>
+      </c>
+      <c r="E35" t="s">
         <v>214</v>
       </c>
-      <c r="D35" t="s">
-        <v>207</v>
-      </c>
-      <c r="E35" t="s">
-        <v>215</v>
-      </c>
       <c r="F35" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1882,16 +1897,16 @@
         <v>84</v>
       </c>
       <c r="C36" t="s">
+        <v>208</v>
+      </c>
+      <c r="D36" t="s">
+        <v>207</v>
+      </c>
+      <c r="E36" t="s">
+        <v>210</v>
+      </c>
+      <c r="F36" t="s">
         <v>209</v>
-      </c>
-      <c r="D36" t="s">
-        <v>208</v>
-      </c>
-      <c r="E36" t="s">
-        <v>211</v>
-      </c>
-      <c r="F36" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1910,16 +1925,16 @@
         <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E38" t="s">
+        <v>215</v>
+      </c>
+      <c r="F38" t="s">
         <v>216</v>
-      </c>
-      <c r="F38" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1930,16 +1945,16 @@
         <v>87</v>
       </c>
       <c r="C39" t="s">
+        <v>218</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E39" t="s">
         <v>219</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E39" t="s">
-        <v>220</v>
-      </c>
       <c r="F39" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1950,16 +1965,16 @@
         <v>88</v>
       </c>
       <c r="C40" t="s">
+        <v>220</v>
+      </c>
+      <c r="D40" t="s">
         <v>221</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
+        <v>223</v>
+      </c>
+      <c r="F40" t="s">
         <v>222</v>
-      </c>
-      <c r="E40" t="s">
-        <v>224</v>
-      </c>
-      <c r="F40" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1973,13 +1988,13 @@
         <v>162</v>
       </c>
       <c r="D41" t="s">
+        <v>224</v>
+      </c>
+      <c r="E41" t="s">
         <v>225</v>
       </c>
-      <c r="E41" t="s">
-        <v>226</v>
-      </c>
       <c r="F41" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1990,10 +2005,10 @@
         <v>90</v>
       </c>
       <c r="E42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2004,16 +2019,16 @@
         <v>91</v>
       </c>
       <c r="C43" t="s">
+        <v>228</v>
+      </c>
+      <c r="D43" t="s">
+        <v>227</v>
+      </c>
+      <c r="E43" t="s">
         <v>229</v>
       </c>
-      <c r="D43" t="s">
-        <v>228</v>
-      </c>
-      <c r="E43" t="s">
-        <v>230</v>
-      </c>
       <c r="F43" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2024,16 +2039,16 @@
         <v>92</v>
       </c>
       <c r="C44" t="s">
+        <v>231</v>
+      </c>
+      <c r="D44" t="s">
+        <v>230</v>
+      </c>
+      <c r="E44" t="s">
+        <v>233</v>
+      </c>
+      <c r="F44" t="s">
         <v>232</v>
-      </c>
-      <c r="D44" t="s">
-        <v>231</v>
-      </c>
-      <c r="E44" t="s">
-        <v>234</v>
-      </c>
-      <c r="F44" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2044,16 +2059,16 @@
         <v>93</v>
       </c>
       <c r="C45" t="s">
+        <v>235</v>
+      </c>
+      <c r="D45" t="s">
+        <v>234</v>
+      </c>
+      <c r="E45" t="s">
+        <v>237</v>
+      </c>
+      <c r="F45" t="s">
         <v>236</v>
-      </c>
-      <c r="D45" t="s">
-        <v>235</v>
-      </c>
-      <c r="E45" t="s">
-        <v>238</v>
-      </c>
-      <c r="F45" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2064,10 +2079,10 @@
         <v>94</v>
       </c>
       <c r="E46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2078,16 +2093,16 @@
         <v>95</v>
       </c>
       <c r="C47" t="s">
+        <v>240</v>
+      </c>
+      <c r="D47" t="s">
         <v>241</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>242</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2098,16 +2113,16 @@
         <v>96</v>
       </c>
       <c r="C48" t="s">
+        <v>256</v>
+      </c>
+      <c r="D48" t="s">
+        <v>255</v>
+      </c>
+      <c r="E48" t="s">
+        <v>258</v>
+      </c>
+      <c r="F48" t="s">
         <v>257</v>
-      </c>
-      <c r="D48" t="s">
-        <v>256</v>
-      </c>
-      <c r="E48" t="s">
-        <v>259</v>
-      </c>
-      <c r="F48" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2118,10 +2133,10 @@
         <v>97</v>
       </c>
       <c r="E49" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F49" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2132,16 +2147,16 @@
         <v>99</v>
       </c>
       <c r="C50" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D50" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E50" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2152,16 +2167,16 @@
         <v>98</v>
       </c>
       <c r="C51" t="s">
+        <v>266</v>
+      </c>
+      <c r="D51" t="s">
+        <v>265</v>
+      </c>
+      <c r="E51" t="s">
+        <v>268</v>
+      </c>
+      <c r="F51" t="s">
         <v>267</v>
-      </c>
-      <c r="D51" t="s">
-        <v>266</v>
-      </c>
-      <c r="E51" t="s">
-        <v>269</v>
-      </c>
-      <c r="F51" t="s">
-        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2180,17 +2195,18 @@
     <hyperlink ref="D15" r:id="rId12" xr:uid="{7BD16280-EE04-D84B-85DA-C4144AB7B5C5}"/>
     <hyperlink ref="F17" r:id="rId13" xr:uid="{5EA871D6-85BA-E247-8CCF-9C0E3F04CD78}"/>
     <hyperlink ref="F19" r:id="rId14" xr:uid="{13B37DFB-F421-F54B-866C-C64E51E576FF}"/>
-    <hyperlink ref="D22" r:id="rId15" location="!/vizhome/WorkforceDevelopmentAreaWDAProfile/WDAProfile" xr:uid="{424EAC4B-0DC5-844B-99DF-C4517C53E9D7}"/>
-    <hyperlink ref="D23" r:id="rId16" xr:uid="{5C3DA8A5-24AE-954A-A955-623114252476}"/>
-    <hyperlink ref="D24" r:id="rId17" xr:uid="{3D071CE2-7D89-2342-878A-991E8909BC45}"/>
-    <hyperlink ref="D29" r:id="rId18" xr:uid="{00DC1C3F-E98A-0344-99BA-92A775EC9AA1}"/>
-    <hyperlink ref="F35" r:id="rId19" xr:uid="{E8845C28-DCDB-5A48-875A-E4C8FE1A2E67}"/>
-    <hyperlink ref="F39" r:id="rId20" xr:uid="{DBD62756-8D96-0641-8C2F-3832F0E94A18}"/>
-    <hyperlink ref="D39" r:id="rId21" xr:uid="{30E97107-CBC0-7446-81D9-0004E9BECB40}"/>
-    <hyperlink ref="F41" r:id="rId22" xr:uid="{5D10423C-2579-804F-9C9C-0B76940BE7A7}"/>
-    <hyperlink ref="F42" r:id="rId23" xr:uid="{65DB9901-F966-0844-A911-CF11F165EC77}"/>
-    <hyperlink ref="F43" r:id="rId24" xr:uid="{59B83F34-8215-944B-872E-08F1229E77D6}"/>
-    <hyperlink ref="D8" r:id="rId25" xr:uid="{CC9E69E5-D89E-7348-94ED-77D234229B97}"/>
+    <hyperlink ref="D23" r:id="rId15" xr:uid="{5C3DA8A5-24AE-954A-A955-623114252476}"/>
+    <hyperlink ref="D24" r:id="rId16" xr:uid="{3D071CE2-7D89-2342-878A-991E8909BC45}"/>
+    <hyperlink ref="D29" r:id="rId17" xr:uid="{00DC1C3F-E98A-0344-99BA-92A775EC9AA1}"/>
+    <hyperlink ref="F35" r:id="rId18" xr:uid="{E8845C28-DCDB-5A48-875A-E4C8FE1A2E67}"/>
+    <hyperlink ref="F39" r:id="rId19" xr:uid="{DBD62756-8D96-0641-8C2F-3832F0E94A18}"/>
+    <hyperlink ref="D39" r:id="rId20" xr:uid="{30E97107-CBC0-7446-81D9-0004E9BECB40}"/>
+    <hyperlink ref="F41" r:id="rId21" xr:uid="{5D10423C-2579-804F-9C9C-0B76940BE7A7}"/>
+    <hyperlink ref="F42" r:id="rId22" xr:uid="{65DB9901-F966-0844-A911-CF11F165EC77}"/>
+    <hyperlink ref="F43" r:id="rId23" xr:uid="{59B83F34-8215-944B-872E-08F1229E77D6}"/>
+    <hyperlink ref="D8" r:id="rId24" xr:uid="{CC9E69E5-D89E-7348-94ED-77D234229B97}"/>
+    <hyperlink ref="D19" r:id="rId25" location="!/vizhome/LWCUIDashboard/DashboardMain" display="https://public.tableau.com/profile/louisiana.workforce.commission.lmi - !/vizhome/LWCUIDashboard/DashboardMain" xr:uid="{8A7AC5E3-4C80-AC4B-BE68-2C22D0A65995}"/>
+    <hyperlink ref="D22" r:id="rId26" location="!/vizhome/InitialClaimsbyCounty_15943981899640/GenderRaceEthnicitybyCounty" display="https://public.tableau.com/profile/maeconomicresearch - !/vizhome/InitialClaimsbyCounty_15943981899640/GenderRaceEthnicitybyCounty" xr:uid="{4E0D811B-0710-DF44-A29A-376C02BA8F74}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update OR to 7/11
</commit_message>
<xml_diff>
--- a/tableau/state_info.xlsx
+++ b/tableau/state_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andy/Documents/GitHub/coronavirus-unemployment/tableau/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0814DCB9-D9DD-D347-8C7A-E8A3F56239EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205D9E43-7FDA-5047-AC79-415751B0FF63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{FAAD1E06-CFD9-6944-82C2-576030DD8CCD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="277">
   <si>
     <t>State</t>
   </si>
@@ -272,9 +272,6 @@
     <t>New Hampshire does not report granular Unemployment Insurance data. Unemployment data is available at the state, county, and city levels.</t>
   </si>
   <si>
-    <t>New Jersey does not report granular Unemployment Insurance data. Unemployment data is available at the state, county, and city levels.</t>
-  </si>
-  <si>
     <t>New Mexico has reported county-level Unemployment Insurance data for April. Unemployment data is available at the state and county levels.</t>
   </si>
   <si>
@@ -861,6 +858,12 @@
   </si>
   <si>
     <t>Department of Unemployment Assistance, Economic Research, Initial Claims by County</t>
+  </si>
+  <si>
+    <t>Unemployment Insurance data for New Jersey is available on a weekly basis. Unemployment data is available at the state, county, and city levels.</t>
+  </si>
+  <si>
+    <t>https://oesc.ok.gov/labor-market-local-area-reports</t>
   </si>
 </sst>
 </file>
@@ -1231,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9EF56E-AA8C-6C43-9629-B47516959724}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1248,19 +1251,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" t="s">
         <v>106</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>107</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>108</v>
-      </c>
-      <c r="F1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1271,16 +1274,16 @@
         <v>51</v>
       </c>
       <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
         <v>102</v>
       </c>
-      <c r="D2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>103</v>
-      </c>
-      <c r="F2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1291,10 +1294,10 @@
         <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1305,16 +1308,16 @@
         <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1325,10 +1328,10 @@
         <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1339,16 +1342,16 @@
         <v>53</v>
       </c>
       <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" t="s">
         <v>115</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1359,16 +1362,16 @@
         <v>54</v>
       </c>
       <c r="C7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" t="s">
         <v>119</v>
       </c>
-      <c r="D7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" t="s">
-        <v>120</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1376,19 +1379,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1399,10 +1402,10 @@
         <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1413,10 +1416,10 @@
         <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1427,16 +1430,16 @@
         <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1447,16 +1450,16 @@
         <v>56</v>
       </c>
       <c r="C12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="D12" t="s">
-        <v>131</v>
-      </c>
-      <c r="E12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1467,16 +1470,16 @@
         <v>58</v>
       </c>
       <c r="C13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" t="s">
         <v>136</v>
-      </c>
-      <c r="D13" t="s">
-        <v>135</v>
-      </c>
-      <c r="E13" t="s">
-        <v>138</v>
-      </c>
-      <c r="F13" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1487,16 +1490,16 @@
         <v>59</v>
       </c>
       <c r="C14" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" t="s">
         <v>140</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>141</v>
-      </c>
-      <c r="F14" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1507,10 +1510,10 @@
         <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1521,16 +1524,16 @@
         <v>60</v>
       </c>
       <c r="C16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" t="s">
         <v>145</v>
-      </c>
-      <c r="D16" t="s">
-        <v>144</v>
-      </c>
-      <c r="E16" t="s">
-        <v>147</v>
-      </c>
-      <c r="F16" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1541,16 +1544,16 @@
         <v>61</v>
       </c>
       <c r="C17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" t="s">
         <v>149</v>
       </c>
-      <c r="D17" t="s">
-        <v>148</v>
-      </c>
-      <c r="E17" t="s">
-        <v>150</v>
-      </c>
       <c r="F17" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1561,16 +1564,16 @@
         <v>62</v>
       </c>
       <c r="C18" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" t="s">
+        <v>153</v>
+      </c>
+      <c r="F18" t="s">
         <v>152</v>
-      </c>
-      <c r="D18" t="s">
-        <v>151</v>
-      </c>
-      <c r="E18" t="s">
-        <v>154</v>
-      </c>
-      <c r="F18" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1581,16 +1584,16 @@
         <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1601,10 +1604,10 @@
         <v>68</v>
       </c>
       <c r="E20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1615,16 +1618,16 @@
         <v>69</v>
       </c>
       <c r="C21" t="s">
+        <v>158</v>
+      </c>
+      <c r="D21" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21" t="s">
+        <v>160</v>
+      </c>
+      <c r="F21" t="s">
         <v>159</v>
-      </c>
-      <c r="D21" t="s">
-        <v>158</v>
-      </c>
-      <c r="E21" t="s">
-        <v>161</v>
-      </c>
-      <c r="F21" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1635,16 +1638,16 @@
         <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1655,16 +1658,16 @@
         <v>71</v>
       </c>
       <c r="C23" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E23" t="s">
+        <v>167</v>
+      </c>
+      <c r="F23" t="s">
         <v>166</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E23" t="s">
-        <v>168</v>
-      </c>
-      <c r="F23" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1675,16 +1678,16 @@
         <v>72</v>
       </c>
       <c r="C24" t="s">
+        <v>169</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E24" t="s">
         <v>170</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="F24" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1695,16 +1698,16 @@
         <v>73</v>
       </c>
       <c r="C25" t="s">
+        <v>172</v>
+      </c>
+      <c r="D25" t="s">
         <v>173</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>175</v>
+      </c>
+      <c r="F25" t="s">
         <v>174</v>
-      </c>
-      <c r="E25" t="s">
-        <v>176</v>
-      </c>
-      <c r="F25" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1715,16 +1718,16 @@
         <v>74</v>
       </c>
       <c r="C26" t="s">
+        <v>176</v>
+      </c>
+      <c r="D26" t="s">
         <v>177</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>178</v>
       </c>
-      <c r="E26" t="s">
-        <v>179</v>
-      </c>
       <c r="F26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1735,10 +1738,10 @@
         <v>75</v>
       </c>
       <c r="E27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1749,16 +1752,16 @@
         <v>76</v>
       </c>
       <c r="C28" t="s">
+        <v>182</v>
+      </c>
+      <c r="D28" t="s">
         <v>183</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
+        <v>185</v>
+      </c>
+      <c r="F28" t="s">
         <v>184</v>
-      </c>
-      <c r="E28" t="s">
-        <v>186</v>
-      </c>
-      <c r="F28" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1769,16 +1772,16 @@
         <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E29" t="s">
+        <v>196</v>
+      </c>
+      <c r="F29" t="s">
         <v>187</v>
-      </c>
-      <c r="E29" t="s">
-        <v>197</v>
-      </c>
-      <c r="F29" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1789,10 +1792,10 @@
         <v>78</v>
       </c>
       <c r="E30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1800,19 +1803,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>79</v>
+        <v>275</v>
       </c>
       <c r="C31" t="s">
+        <v>190</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E31" t="s">
         <v>191</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E31" t="s">
-        <v>192</v>
-      </c>
       <c r="F31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1820,19 +1823,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
+        <v>192</v>
+      </c>
+      <c r="D32" t="s">
         <v>193</v>
       </c>
-      <c r="D32" t="s">
-        <v>194</v>
-      </c>
       <c r="E32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1840,19 +1843,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D33" t="s">
+        <v>199</v>
+      </c>
+      <c r="E33" t="s">
+        <v>203</v>
+      </c>
+      <c r="F33" t="s">
         <v>200</v>
-      </c>
-      <c r="E33" t="s">
-        <v>204</v>
-      </c>
-      <c r="F33" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1860,13 +1863,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1874,19 +1877,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
+        <v>212</v>
+      </c>
+      <c r="D35" t="s">
+        <v>205</v>
+      </c>
+      <c r="E35" t="s">
         <v>213</v>
       </c>
-      <c r="D35" t="s">
-        <v>206</v>
-      </c>
-      <c r="E35" t="s">
-        <v>214</v>
-      </c>
       <c r="F35" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1894,19 +1897,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" t="s">
+        <v>206</v>
+      </c>
+      <c r="E36" t="s">
+        <v>209</v>
+      </c>
+      <c r="F36" t="s">
         <v>208</v>
-      </c>
-      <c r="D36" t="s">
-        <v>207</v>
-      </c>
-      <c r="E36" t="s">
-        <v>210</v>
-      </c>
-      <c r="F36" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1914,7 +1917,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1922,19 +1928,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E38" t="s">
+        <v>214</v>
+      </c>
+      <c r="F38" t="s">
         <v>215</v>
-      </c>
-      <c r="F38" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1942,19 +1948,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C39" t="s">
+        <v>217</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E39" t="s">
         <v>218</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E39" t="s">
-        <v>219</v>
-      </c>
       <c r="F39" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1962,19 +1968,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C40" t="s">
+        <v>219</v>
+      </c>
+      <c r="D40" t="s">
         <v>220</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
+        <v>222</v>
+      </c>
+      <c r="F40" t="s">
         <v>221</v>
-      </c>
-      <c r="E40" t="s">
-        <v>223</v>
-      </c>
-      <c r="F40" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1982,19 +1988,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E41" t="s">
         <v>224</v>
       </c>
-      <c r="E41" t="s">
-        <v>225</v>
-      </c>
       <c r="F41" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2002,13 +2008,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2016,19 +2022,19 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C43" t="s">
+        <v>227</v>
+      </c>
+      <c r="D43" t="s">
+        <v>226</v>
+      </c>
+      <c r="E43" t="s">
         <v>228</v>
       </c>
-      <c r="D43" t="s">
-        <v>227</v>
-      </c>
-      <c r="E43" t="s">
-        <v>229</v>
-      </c>
       <c r="F43" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2036,19 +2042,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
+        <v>230</v>
+      </c>
+      <c r="D44" t="s">
+        <v>229</v>
+      </c>
+      <c r="E44" t="s">
+        <v>232</v>
+      </c>
+      <c r="F44" t="s">
         <v>231</v>
-      </c>
-      <c r="D44" t="s">
-        <v>230</v>
-      </c>
-      <c r="E44" t="s">
-        <v>233</v>
-      </c>
-      <c r="F44" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2056,19 +2062,19 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C45" t="s">
+        <v>234</v>
+      </c>
+      <c r="D45" t="s">
+        <v>233</v>
+      </c>
+      <c r="E45" t="s">
+        <v>236</v>
+      </c>
+      <c r="F45" t="s">
         <v>235</v>
-      </c>
-      <c r="D45" t="s">
-        <v>234</v>
-      </c>
-      <c r="E45" t="s">
-        <v>237</v>
-      </c>
-      <c r="F45" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2076,13 +2082,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F46" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2090,19 +2096,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C47" t="s">
+        <v>239</v>
+      </c>
+      <c r="D47" t="s">
         <v>240</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>241</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2110,19 +2116,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
+        <v>255</v>
+      </c>
+      <c r="D48" t="s">
+        <v>254</v>
+      </c>
+      <c r="E48" t="s">
+        <v>257</v>
+      </c>
+      <c r="F48" t="s">
         <v>256</v>
-      </c>
-      <c r="D48" t="s">
-        <v>255</v>
-      </c>
-      <c r="E48" t="s">
-        <v>258</v>
-      </c>
-      <c r="F48" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2130,13 +2136,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E49" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F49" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2144,19 +2150,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C50" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D50" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F50" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2164,19 +2170,19 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C51" t="s">
+        <v>265</v>
+      </c>
+      <c r="D51" t="s">
+        <v>264</v>
+      </c>
+      <c r="E51" t="s">
+        <v>267</v>
+      </c>
+      <c r="F51" t="s">
         <v>266</v>
-      </c>
-      <c r="D51" t="s">
-        <v>265</v>
-      </c>
-      <c r="E51" t="s">
-        <v>268</v>
-      </c>
-      <c r="F51" t="s">
-        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -2207,7 +2213,9 @@
     <hyperlink ref="D8" r:id="rId24" xr:uid="{CC9E69E5-D89E-7348-94ED-77D234229B97}"/>
     <hyperlink ref="D19" r:id="rId25" location="!/vizhome/LWCUIDashboard/DashboardMain" display="https://public.tableau.com/profile/louisiana.workforce.commission.lmi - !/vizhome/LWCUIDashboard/DashboardMain" xr:uid="{8A7AC5E3-4C80-AC4B-BE68-2C22D0A65995}"/>
     <hyperlink ref="D22" r:id="rId26" location="!/vizhome/InitialClaimsbyCounty_15943981899640/GenderRaceEthnicitybyCounty" display="https://public.tableau.com/profile/maeconomicresearch - !/vizhome/InitialClaimsbyCounty_15943981899640/GenderRaceEthnicitybyCounty" xr:uid="{4E0D811B-0710-DF44-A29A-376C02BA8F74}"/>
+    <hyperlink ref="F37" r:id="rId27" xr:uid="{C448FDF3-45E9-B24C-9FC6-786BC4936749}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>